<commit_message>
everything works, job's done. but it is only sashimi now
</commit_message>
<xml_diff>
--- a/feedbacks.xlsx
+++ b/feedbacks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -731,6 +731,316 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ольга</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>89865</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>22.02.2023</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Нет, сегодня впервые рисовала👍</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>запомнили основные правила и технику безопасности для экологичного рисования</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Вопрос</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Воодушевление, уверенность, спокойствие</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Отзыв</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Увеличение дохода</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Булат</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8965</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Мораль 22.03.2023</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Рисовала на бесплатном марафоне😁</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>запомнили основные правила и технику безопасности для экологичного рисования</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Всё понятно!</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Напряжение усилилось</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Нормас</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Здоровье</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bulat</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11233</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Fhjj</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Рисовала другой алгоритм на очном МК</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>вошли в состояние медитации, появилось ощущение гармонии</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Всё понятно!</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Воодушевление, уверенность, спокойствие</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Hhh</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Рост в профессии</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Рисовала на бесплатном марафоне😁</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>просто получили удовольствие от процесса</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Всё понятно!</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Напряжение усилилось</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>рпоп</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Переезд</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>but</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>wad</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>wad</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>wqedas</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Рисовала другой алгоритм на очном МК</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>просто получили удовольствие от процесса</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Всё понятно!</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Хорошее настроение,вдохновение</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>qwsA</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Отношения с детьми</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>